<commit_message>
fixed full cycle test
</commit_message>
<xml_diff>
--- a/tests/Answer_stud1_NOT_PLAGIARISED.xlsx
+++ b/tests/Answer_stud1_NOT_PLAGIARISED.xlsx
@@ -192,7 +192,7 @@
       <selection pane="topLeft" activeCell="KE4423" activeCellId="0" sqref="KE4423"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.66"/>
   </cols>
@@ -263,10 +263,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -287,7 +287,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>11684</v>
+        <v>4951</v>
       </c>
     </row>
   </sheetData>

</xml_diff>